<commit_message>
Add roles to Alexion study
</commit_message>
<xml_diff>
--- a/source_data/protocols/NCT04573309_Alexion_Wilsons/NCT04573309.xlsx
+++ b/source_data/protocols/NCT04573309_Alexion_Wilsons/NCT04573309.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/NCT04573309/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/NCT04573309_Alexion_Wilsons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0963B5-B5A1-AC4B-BF9B-801183C69D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D527A5E2-9D32-A942-B127-614B9AA4C938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36400" yWindow="500" windowWidth="36400" windowHeight="19900" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36400" yWindow="500" windowWidth="36400" windowHeight="19900" firstSheet="20" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -38,19 +38,20 @@
     <sheet name="studyDesignProcedures" sheetId="23" r:id="rId23"/>
     <sheet name="studyDesignEncounters" sheetId="24" r:id="rId24"/>
     <sheet name="studyDesignElements" sheetId="25" r:id="rId25"/>
-    <sheet name="dictionaries" sheetId="26" r:id="rId26"/>
-    <sheet name="documentContent" sheetId="28" r:id="rId27"/>
-    <sheet name="document" sheetId="29" r:id="rId28"/>
-    <sheet name="abbreviations" sheetId="32" r:id="rId29"/>
-    <sheet name="notes" sheetId="33" r:id="rId30"/>
-    <sheet name="configuration" sheetId="27" r:id="rId31"/>
+    <sheet name="roles" sheetId="51" r:id="rId26"/>
+    <sheet name="abbreviations" sheetId="32" r:id="rId27"/>
+    <sheet name="notes" sheetId="33" r:id="rId28"/>
+    <sheet name="dictionaries" sheetId="26" r:id="rId29"/>
+    <sheet name="documentContent" sheetId="28" r:id="rId30"/>
+    <sheet name="document" sheetId="29" r:id="rId31"/>
+    <sheet name="configuration" sheetId="27" r:id="rId32"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3536" uniqueCount="1627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3549" uniqueCount="1634">
   <si>
     <t>name</t>
   </si>
@@ -7072,6 +7073,27 @@
   </si>
   <si>
     <t>This is a parent activity</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>organizations</t>
+  </si>
+  <si>
+    <t>ROLE_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masked </t>
+  </si>
+  <si>
+    <t>Sponsor role</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
+  </si>
+  <si>
+    <t>sponsor</t>
   </si>
 </sst>
 </file>
@@ -7373,15 +7395,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -11457,7 +11479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="B35" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
@@ -14163,6 +14185,288 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF7CA68-BC48-5141-BEA0-B0ABEF929D94}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="7" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>815</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1630</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1633</v>
+      </c>
+      <c r="G2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436F4EB7-AE9E-884E-85DF-B96833175199}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82933AAF-F060-9544-8A9A-79B341EF929B}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="72.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -14231,7 +14535,147 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="62.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D106"/>
   <sheetViews>
@@ -14278,7 +14722,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1055</v>
       </c>
@@ -14569,7 +15013,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="272" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="256" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>1125</v>
       </c>
@@ -14593,7 +15037,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>1131</v>
       </c>
@@ -15085,7 +15529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:F106"/>
   <sheetViews>
@@ -17229,365 +17673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436F4EB7-AE9E-884E-85DF-B96833175199}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
-        <v>1602</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>1603</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1604</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>482</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1570</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1572</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1576</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>1578</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1579</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1580</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1581</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1582</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1584</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>1586</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>1588</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1590</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>1592</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>1594</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1595</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1596</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>1598</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1599</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>1600</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1601</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="62.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82933AAF-F060-9544-8A9A-79B341EF929B}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="72.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>141</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1622</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1626</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1624</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -17656,144 +17742,144 @@
       <c r="A1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
       <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -17841,11 +17927,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B10:E10"/>
@@ -17853,6 +17934,11 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>